<commit_message>
kevin time log update
</commit_message>
<xml_diff>
--- a/docs/time_logs/kevin_time_log.xlsx
+++ b/docs/time_logs/kevin_time_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\netbsd-wifi-browser\docs\time_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B7DDB4-E3BA-41E5-AA9B-D0D043278EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2B6981-32A7-49F8-A3A8-E83CAB8CE31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Name Here</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Milestone 4 work</t>
+  </si>
+  <si>
+    <t>TUI Implementation</t>
+  </si>
+  <si>
+    <t>Practice with sub-windows in Ncurses</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -594,7 +600,7 @@
         <v>44210.625</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ref="C7:C27" si="1">B7-A7</f>
+        <f t="shared" ref="C7:C29" si="1">B7-A7</f>
         <v>4.1666666664241347E-2</v>
       </c>
       <c r="D7" s="5">
@@ -636,7 +642,7 @@
         <v>4.1666666671517305E-2</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" ref="D9:D27" si="2">C9+D8</f>
+        <f t="shared" ref="D9:D29" si="2">C9+D8</f>
         <v>0.13541666666424135</v>
       </c>
       <c r="E9" t="s">
@@ -983,6 +989,82 @@
       </c>
       <c r="E27" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>44620.708333333336</v>
+      </c>
+      <c r="B28" s="7">
+        <v>44620.770833333336</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="2"/>
+        <v>0.70833333332848269</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>44621.416666666664</v>
+      </c>
+      <c r="B29" s="7">
+        <v>44621.447916666664</v>
+      </c>
+      <c r="C29" s="5">
+        <f>B29-A29</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D29" s="5">
+        <f>C29+D28</f>
+        <v>0.73958333332848269</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>44622.416666666664</v>
+      </c>
+      <c r="B30" s="7">
+        <v>44622.427083333336</v>
+      </c>
+      <c r="C30" s="5">
+        <f>B30-A30</f>
+        <v>1.0416666671517305E-2</v>
+      </c>
+      <c r="D30" s="5">
+        <f>C30+D29</f>
+        <v>0.75</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>44622.583333333336</v>
+      </c>
+      <c r="B31" s="7">
+        <v>44622.59375</v>
+      </c>
+      <c r="C31" s="5">
+        <f>B31-A31</f>
+        <v>1.0416666664241347E-2</v>
+      </c>
+      <c r="D31" s="5">
+        <f>C31+D30</f>
+        <v>0.76041666666424135</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kevin time logs update
</commit_message>
<xml_diff>
--- a/docs/time_logs/kevin_time_log.xlsx
+++ b/docs/time_logs/kevin_time_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\netbsd-wifi-browser\docs\time_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2B6981-32A7-49F8-A3A8-E83CAB8CE31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09798DF-BF36-4987-AE5D-15594538124A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1680" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Name Here</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Practice with sub-windows in Ncurses</t>
+  </si>
+  <si>
+    <t>Milestone 5 work</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -600,7 +603,7 @@
         <v>44210.625</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ref="C7:C29" si="1">B7-A7</f>
+        <f t="shared" ref="C7:C28" si="1">B7-A7</f>
         <v>4.1666666664241347E-2</v>
       </c>
       <c r="D7" s="5">
@@ -642,7 +645,7 @@
         <v>4.1666666671517305E-2</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" ref="D9:D29" si="2">C9+D8</f>
+        <f t="shared" ref="D9:D28" si="2">C9+D8</f>
         <v>0.13541666666424135</v>
       </c>
       <c r="E9" t="s">
@@ -1065,6 +1068,25 @@
       </c>
       <c r="E31" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>44631</v>
+      </c>
+      <c r="B32" s="7">
+        <v>44631.041666666664</v>
+      </c>
+      <c r="C32" s="5">
+        <f>B32-A32</f>
+        <v>4.1666666664241347E-2</v>
+      </c>
+      <c r="D32" s="5">
+        <f>C32+D31</f>
+        <v>0.80208333332848269</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>